<commit_message>
Refactor configuration management and enhance utility bill processing
- Updated `config.py` to streamline configuration loading with fallbacks and added tenant data defaults.
- Introduced new data processing functions in `data_processing.py` for improved normalization and vendor detection.
- Consolidated PDF extraction logic into `bill_extractors.py` and removed redundant files.
- Added utility functions for email draft generation and improved handling of vendor-specific data.
- Created new documentation files: `instructions.md` and `workflow.md` for user guidance on processing utility bills.
- Updated `main.py` to reflect changes in data handling and email generation logic.
</commit_message>
<xml_diff>
--- a/utility_bills.xlsx
+++ b/utility_bills.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Config" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Config (2)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Tenants" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Tenants" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,8 +18,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -79,12 +78,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -93,9 +91,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +451,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1705 August 26 2025 ENMAX.pdf</t>
+          <t>1705 August 20 2025 ATCO.PDF</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -469,41 +469,41 @@
         <v>60</v>
       </c>
       <c r="F2" t="n">
-        <v>179.97</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>45895</v>
+        <v>217.59</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>45889</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ENMAX</t>
+          <t>ATCO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1707 August 26 2025 ENMAX.pdf</t>
+          <t>1705 August 26 2025 ENMAX.pdf</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1707_tenant</t>
+          <t>1705_tenant</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="E3" t="n">
         <v>60</v>
       </c>
       <c r="F3" t="n">
-        <v>135.49</v>
-      </c>
-      <c r="G3" s="2" t="n">
+        <v>179.97</v>
+      </c>
+      <c r="G3" s="8" t="n">
         <v>45895</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -515,60 +515,60 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1712 August 26 2025 ENMAX.pdf</t>
+          <t>1707 August 20 2025 ATCO.PDF</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1712</v>
+        <v>1707</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1712_tenant</t>
+          <t>1707_tenant</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1712</v>
+        <v>1707</v>
       </c>
       <c r="E4" t="n">
         <v>60</v>
       </c>
       <c r="F4" t="n">
-        <v>322.5</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>45895</v>
+        <v>177.2</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>45889</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ENMAX</t>
+          <t>ATCO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>819 August 25 2025 ENMAX.pdf</t>
+          <t>1707 August 26 2025 ENMAX.pdf</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>819</v>
+        <v>1707</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>819_tenant</t>
+          <t>1707_tenant</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>819</v>
+        <v>1707</v>
       </c>
       <c r="E5" t="n">
         <v>60</v>
       </c>
       <c r="F5" t="n">
-        <v>324.48</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>45894</v>
+        <v>135.49</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>45895</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -579,64 +579,64 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1705 August 20 2025 ATCO.PDF</t>
+          <t>1712 August 26 2025 ENMAX.pdf</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1705</v>
+        <v>1712</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1705_tenant</t>
+          <t>1712_tenant</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1705</v>
+        <v>1712</v>
       </c>
       <c r="E6" t="n">
         <v>60</v>
       </c>
       <c r="F6" t="n">
-        <v>217.59</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>45889</v>
+        <v>322.5</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>45895</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ATCO</t>
+          <t>ENMAX</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1707 August 20 2025 ATCO.PDF</t>
+          <t>819 August 25 2025 ENMAX.pdf</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1707</v>
+        <v>819</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1707_tenant</t>
+          <t>819_tenant</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1707</v>
+        <v>819</v>
       </c>
       <c r="E7" t="n">
         <v>60</v>
       </c>
       <c r="F7" t="n">
-        <v>177.2</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>45889</v>
+        <v>324.48</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>45894</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>ATCO</t>
+          <t>ENMAX</t>
         </is>
       </c>
     </row>
@@ -651,31 +651,31 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="100" workbookViewId="0">
       <selection activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="21.1640625" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="40.75" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="44.58203125" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="21.1640625" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="40.75" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="69.7109375" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>key</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>value</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -687,14 +687,14 @@
           <t>excel_data_sheet</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Name of the Excel sheet containing bill data</t>
+          <t>Excel sheet name where processed bill data is stored</t>
         </is>
       </c>
     </row>
@@ -704,10 +704,14 @@
           <t>raw_bills_folder</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n"/>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>bills</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Folder where raw PDF bills are downloaded</t>
+          <t>Folder path where you place PDF bills to be processed (input folder)</t>
         </is>
       </c>
     </row>
@@ -717,10 +721,14 @@
           <t>processed_bills_folder</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>bills_processed</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Folder where processed PDFs are moved</t>
+          <t>Folder path where processed PDF bills are moved after processing (output folder)</t>
         </is>
       </c>
     </row>
@@ -730,10 +738,14 @@
           <t>images_folder</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n"/>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>bill_images</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Folder where bill images are saved</t>
+          <t>Folder path where PNG images of bill pages are saved for email attachments</t>
         </is>
       </c>
     </row>
@@ -743,12 +755,14 @@
           <t>image_bottom_crop_px</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>450</v>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pixels to crop from bottom of images</t>
+          <t>Number of pixels to crop from bottom of bill images (removes footers/ads)</t>
         </is>
       </c>
     </row>
@@ -758,14 +772,14 @@
           <t>atco_indicator</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>statements</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>String in filename that indicates ATCO vendor</t>
+          <t>Keyword in filename that identifies ATCO bills (vs ENMAX bills)</t>
         </is>
       </c>
     </row>
@@ -775,29 +789,48 @@
           <t>house_numbers</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>819,1705,1707,1712</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Comma-separated list of house numbers</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+          <t>Comma-separated list of property addresses to extract from bills</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1" s="2">
       <c r="A9" t="inlineStr">
         <is>
           <t>move_processed_files</t>
         </is>
       </c>
-      <c r="B9" s="4" t="b">
-        <v>1</v>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Whether to move files after processing (True/False)</t>
+          <t>Whether to move PDF files to processed folder after extraction (True/False)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" s="2">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test_email_drafts</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Prints emails instead of creating drafts when TRUE</t>
         </is>
       </c>
     </row>
@@ -814,214 +847,39 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="B9" activeCellId="0" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
-  <cols>
-    <col width="21.1640625" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="40.75" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
-    <col width="44.58203125" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>key</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>excel_data_sheet</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Name of the Excel sheet containing bill data</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>raw_bills_folder</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>D:/Rental Project/rental/bills</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Folder where raw PDF bills are downloaded</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>processed_bills_folder</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>D:/Rental Project/rental/bills_processed</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Folder where processed PDFs are moved</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>images_folder</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>D:/Rental Project/rental/bill_images</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Folder where bill images are saved</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>image_bottom_crop_px</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>450</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Pixels to crop from bottom of images</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>atco_indicator</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>statements</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>String in filename that indicates ATCO vendor</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>house_numbers</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>819,1705,1707,1712</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Comma-separated list of house numbers</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>move_processed_files</t>
-        </is>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Whether to move files after processing (True/False)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" useFirstPageNumber="0" pageOrder="downThenOver" usePrinterDefaults="1" blackAndWhite="0" draft="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="25" customWidth="1" style="3" min="2" max="2"/>
+    <col width="25" customWidth="1" style="2" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>house_number</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>tenant_name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>base_rent</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>utility_share_percent</t>
         </is>

</xml_diff>